<commit_message>
All mesures done + plots for all problems
</commit_message>
<xml_diff>
--- a/P3/Reports/Data.xlsx
+++ b/P3/Reports/Data.xlsx
@@ -648,7 +648,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,6 +927,21 @@
       <c r="C11">
         <v>10</v>
       </c>
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>13</v>
+      </c>
+      <c r="F11">
+        <v>50</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <v>0.89939999999999998</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1142,6 +1157,21 @@
       <c r="C21">
         <v>10</v>
       </c>
+      <c r="D21">
+        <v>86</v>
+      </c>
+      <c r="E21">
+        <v>88</v>
+      </c>
+      <c r="F21">
+        <v>841</v>
+      </c>
+      <c r="G21">
+        <v>9</v>
+      </c>
+      <c r="H21">
+        <v>149.0453</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -1341,6 +1371,21 @@
       </c>
       <c r="C31">
         <v>10</v>
+      </c>
+      <c r="D31">
+        <v>316</v>
+      </c>
+      <c r="E31">
+        <v>318</v>
+      </c>
+      <c r="F31">
+        <v>2912</v>
+      </c>
+      <c r="G31">
+        <v>12</v>
+      </c>
+      <c r="H31">
+        <v>764.67840000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>